<commit_message>
PROS-9303 - CCRU - Wrong KPI calculation. NCB Display
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/PoS 2019 - MT Conv Big - CAP.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/PoS 2019 - MT Conv Big - CAP.xlsx
@@ -16,6 +16,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Conv_B_CAP!$A$1:$AM$191</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Conv_B_CAP!$A$1:$AM$191</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Conv_B_CAP!$A$1:$AM$191</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Conv_B_CAP!$A$1:$AM$191</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1323,7 +1324,7 @@
     <t xml:space="preserve">NCB Дисплей: Фейсинги</t>
   </si>
   <si>
-    <t xml:space="preserve">ice tea, water</t>
+    <t xml:space="preserve">ice tea, Water</t>
   </si>
   <si>
     <t xml:space="preserve">NCB Display: Zone</t>
@@ -2451,52 +2452,51 @@
   <dimension ref="A1:AM191"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F104" activeCellId="0" sqref="F104:AM104"/>
+      <selection pane="bottomLeft" activeCell="N128" activeCellId="0" sqref="N128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1376518218623"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.9878542510121"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="68.3400809716599"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="50.2388663967611"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.417004048583"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="68.8785425101215"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="50.668016194332"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.6032388663968"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="60.417004048583"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="64.0566801619433"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="60.9514170040486"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="64.7004048582996"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="20.246963562753"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="87.5141700404858"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="126.291497975708"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="55.914979757085"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="88.3724696356275"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="127.46963562753"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="56.3441295546559"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="27.4210526315789"/>
     <col collapsed="false" hidden="false" max="29" min="29" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="17.5668016194332"/>
     <col collapsed="false" hidden="false" max="31" min="31" style="0" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="95.9797570850202"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="33" min="32" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="96.834008097166"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="22.7085020242915"/>
     <col collapsed="false" hidden="false" max="36" min="36" style="0" width="7.92712550607287"/>
     <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="38" min="38" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="10.0688259109312"/>
     <col collapsed="false" hidden="false" max="1025" min="40" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>